<commit_message>
Added support for metadata
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoclient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F6C397-7809-4AFA-81D1-AC5F654EC814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D15C24-EBEC-4199-8355-5AEA3BC2DF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="2" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
   <sheets>
     <sheet name="Zuordnung" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="117">
   <si>
     <t>Person*</t>
   </si>
@@ -1061,7 +1061,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="G2" sqref="G2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2142,24 +2142,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D57FB1A-6D98-4995-87AD-13E81E29DC39}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="12.53515625" customWidth="1"/>
     <col min="4" max="4" width="17.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.07421875" customWidth="1"/>
+    <col min="6" max="6" width="24.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -2175,8 +2177,11 @@
       <c r="E3" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F3" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2192,8 +2197,11 @@
       <c r="E4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2209,8 +2217,11 @@
       <c r="E5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2226,13 +2237,44 @@
       <c r="E6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
         <v>70</v>
       </c>
       <c r="E7" t="s">
         <v>74</v>
+      </c>
+      <c r="F7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="F12" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2244,7 +2286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E40AA6-B7EF-45C8-9C99-020982588CCB}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added CIRP activity to metadata
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoclient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D15C24-EBEC-4199-8355-5AEA3BC2DF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020017A2-8125-4C16-AE9A-948DDEACC543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
   <sheets>
     <sheet name="Zuordnung" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="121">
   <si>
     <t>Person*</t>
   </si>
@@ -495,6 +495,18 @@
   </si>
   <si>
     <t>0.0.1</t>
+  </si>
+  <si>
+    <t>CIRP Activity</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>Tool Wear Monitoring</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1073,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:O2"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1421,6 +1433,50 @@
         <v>28</v>
       </c>
     </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="13" t="s">
         <v>4</v>
@@ -2114,7 +2170,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:F1048576">
+  <conditionalFormatting sqref="D2:F1048576 H9:J9">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="suggestions">
       <formula>NOT(ISERROR(SEARCH("suggestions",D2)))</formula>
     </cfRule>
@@ -2142,10 +2198,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D57FB1A-6D98-4995-87AD-13E81E29DC39}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2154,14 +2210,15 @@
     <col min="4" max="4" width="17.3828125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.07421875" customWidth="1"/>
     <col min="6" max="6" width="24.69140625" customWidth="1"/>
+    <col min="7" max="7" width="19.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -2180,8 +2237,11 @@
       <c r="F3" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G3" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2200,8 +2260,11 @@
       <c r="F4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2221,7 +2284,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2241,7 +2304,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D7" t="s">
         <v>70</v>
       </c>
@@ -2252,27 +2315,27 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F12" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Update to metadata: coolant & institutions
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoclient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020017A2-8125-4C16-AE9A-948DDEACC543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1951B915-5213-4B3F-A119-C8FB05DF991A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="122">
   <si>
     <t>Person*</t>
   </si>
@@ -248,9 +248,6 @@
     <t>MMQ</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>Machine</t>
   </si>
   <si>
@@ -341,24 +338,9 @@
     <t>TU Wien</t>
   </si>
   <si>
-    <t>TU München</t>
-  </si>
-  <si>
-    <t>ETH Zürich</t>
-  </si>
-  <si>
     <t>workpiece_material</t>
   </si>
   <si>
-    <t>S235</t>
-  </si>
-  <si>
-    <t>TiAl</t>
-  </si>
-  <si>
-    <t>Grade 5 Titanium</t>
-  </si>
-  <si>
     <t>Carbide</t>
   </si>
   <si>
@@ -507,6 +489,27 @@
   </si>
   <si>
     <t>Tool Wear Monitoring</t>
+  </si>
+  <si>
+    <t>Dry</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>TU Darmstadt</t>
+  </si>
+  <si>
+    <t>C45</t>
+  </si>
+  <si>
+    <t>Steel (generic)</t>
+  </si>
+  <si>
+    <t>Carbide (P40)</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1076,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1138,31 +1141,31 @@
         <v>18</v>
       </c>
       <c r="G2" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="N2" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="O2" s="20" t="s">
         <v>105</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.45">
@@ -1179,37 +1182,37 @@
         <v>23</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="N3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
@@ -1220,14 +1223,14 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>28</v>
@@ -1265,13 +1268,13 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
@@ -1306,16 +1309,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>28</v>
@@ -1350,16 +1353,16 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>28</v>
@@ -1394,16 +1397,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>28</v>
@@ -1435,19 +1438,19 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="13" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>28</v>
@@ -1482,16 +1485,16 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>28</v>
@@ -1526,19 +1529,19 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>28</v>
@@ -1573,19 +1576,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>28</v>
@@ -1617,22 +1620,22 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>30</v>
@@ -1667,19 +1670,19 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>28</v>
@@ -1714,19 +1717,19 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>28</v>
@@ -1758,22 +1761,22 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>30</v>
@@ -1805,22 +1808,22 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17" s="16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>90</v>
-      </c>
       <c r="F17" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>30</v>
@@ -1855,19 +1858,19 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>28</v>
@@ -1902,17 +1905,17 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>28</v>
@@ -1947,17 +1950,17 @@
         <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>28</v>
@@ -1992,19 +1995,19 @@
         <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>28</v>
@@ -2042,14 +2045,14 @@
         <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>28</v>
@@ -2084,17 +2087,17 @@
         <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>28</v>
@@ -2129,17 +2132,17 @@
         <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>28</v>
@@ -2201,12 +2204,13 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="12.53515625" customWidth="1"/>
+    <col min="3" max="3" width="12.23046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.3828125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.07421875" customWidth="1"/>
     <col min="6" max="6" width="24.69140625" customWidth="1"/>
@@ -2223,22 +2227,22 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -2246,22 +2250,22 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -2269,19 +2273,19 @@
         <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
         <v>65</v>
       </c>
-      <c r="D5">
-        <v>4140</v>
-      </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -2289,55 +2293,55 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
         <v>66</v>
       </c>
-      <c r="D6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" t="s">
-        <v>72</v>
-      </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="D7" t="s">
-        <v>70</v>
+      <c r="B7" t="s">
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
       <c r="F8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F12" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2357,10 +2361,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Updated metadata according to CIRP TWM experiments
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D04D09-90D9-4016-B461-922560E753A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48387402-4FAA-46A8-8AD8-687B4F02661E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="6" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="7" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="post_milling" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -549,90 +550,6 @@
     <t>Tool Breakage</t>
   </si>
   <si>
-    <t>primary_ce</t>
-  </si>
-  <si>
-    <t>secondary_ce</t>
-  </si>
-  <si>
-    <t>Primary Cutting Edge</t>
-  </si>
-  <si>
-    <t>Secondary Cutting Edge</t>
-  </si>
-  <si>
-    <t>primary_wear_mark_width</t>
-  </si>
-  <si>
-    <t>primary_max_wear_mark_width</t>
-  </si>
-  <si>
-    <t>secondary_wear_mark_width</t>
-  </si>
-  <si>
-    <t>secondary_max_wear_mark_width</t>
-  </si>
-  <si>
-    <t>primary_tool_wear_exceeded</t>
-  </si>
-  <si>
-    <t>Tool Wear Exceeded (Primary CE)</t>
-  </si>
-  <si>
-    <t>secondary_tool_wear_exceeded</t>
-  </si>
-  <si>
-    <t>Tool Wear Exceeded (Secondary CE)</t>
-  </si>
-  <si>
-    <t>Avg. Wear Mark Width (Primary CE)</t>
-  </si>
-  <si>
-    <t>Avg. Wear Mark Width (Secondary CE)</t>
-  </si>
-  <si>
-    <t>Max. Wear Mark Width (Primary CE)</t>
-  </si>
-  <si>
-    <t>Max. Wear Mark Width (Secondary CE)</t>
-  </si>
-  <si>
-    <t>Measured avg. width of the wear mark on the primary cutting edge</t>
-  </si>
-  <si>
-    <t>Measured max. width of the wear mark on the primary cutting edge</t>
-  </si>
-  <si>
-    <t>Has the tool exceeded the maximum wear on the primary cutting edge?</t>
-  </si>
-  <si>
-    <t>Measured avg. width of the wear mark on the secondary cutting edge</t>
-  </si>
-  <si>
-    <t>Measured max. width of the wear mark on the secondary cutting edge</t>
-  </si>
-  <si>
-    <t>Has the tool exceeded the maximum wear on the secondary cutting edge?</t>
-  </si>
-  <si>
-    <t>primary_pictures</t>
-  </si>
-  <si>
-    <t>secondary_pictures</t>
-  </si>
-  <si>
-    <t>Pictures of Primary Cutting Edge</t>
-  </si>
-  <si>
-    <t>Pictures of Secondary Cutting Edge</t>
-  </si>
-  <si>
-    <t>Pictures of the primary cutting edge</t>
-  </si>
-  <si>
-    <t>Pictures of the secondary cutting edge</t>
-  </si>
-  <si>
     <t>twm_cirp_tool2</t>
   </si>
   <si>
@@ -640,6 +557,90 @@
   </si>
   <si>
     <t>CIRP TWM 2 (ae=10mm)</t>
+  </si>
+  <si>
+    <t>first_tool_wear_exceeded</t>
+  </si>
+  <si>
+    <t>first_wear_mark_width</t>
+  </si>
+  <si>
+    <t>first_max_wear_mark_width</t>
+  </si>
+  <si>
+    <t>first_pictures</t>
+  </si>
+  <si>
+    <t>Tool Wear Exceeded (First Peripheral CE)</t>
+  </si>
+  <si>
+    <t>Avg. Wear Mark Width (First Peripheral CE)</t>
+  </si>
+  <si>
+    <t>Max. Wear Mark Width (First Peripheral CE)</t>
+  </si>
+  <si>
+    <t>Pictures of First Peripheral Cutting Edge</t>
+  </si>
+  <si>
+    <t>second_wear_mark_width</t>
+  </si>
+  <si>
+    <t>second_max_wear_mark_width</t>
+  </si>
+  <si>
+    <t>second_tool_wear_exceeded</t>
+  </si>
+  <si>
+    <t>second_pictures</t>
+  </si>
+  <si>
+    <t>Avg. Wear Mark Width (Second Peripheral CE)</t>
+  </si>
+  <si>
+    <t>Max. Wear Mark Width (Second Peripheral CE)</t>
+  </si>
+  <si>
+    <t>Tool Wear Exceeded (Second Peripheral CE)</t>
+  </si>
+  <si>
+    <t>Pictures of Second Peripheral Cutting Edge</t>
+  </si>
+  <si>
+    <t>first_ce</t>
+  </si>
+  <si>
+    <t>second_ce</t>
+  </si>
+  <si>
+    <t>First Cutting Edge</t>
+  </si>
+  <si>
+    <t>Second Cutting Edge</t>
+  </si>
+  <si>
+    <t>Measured avg. width of the wear mark on the first peripheral cutting edge</t>
+  </si>
+  <si>
+    <t>Measured max. width of the wear mark on the first peripheral cutting edge</t>
+  </si>
+  <si>
+    <t>Has the tool exceeded the maximum wear on the first peripheral cutting edge?</t>
+  </si>
+  <si>
+    <t>Pictures of the first peripheral cutting edge</t>
+  </si>
+  <si>
+    <t>Measured avg. width of the wear mark on the second peripheral cutting edge</t>
+  </si>
+  <si>
+    <t>Measured max. width of the wear mark on the second peripheral cutting edge</t>
+  </si>
+  <si>
+    <t>Has the tool exceeded the maximum wear on the second peripheral cutting edge?</t>
+  </si>
+  <si>
+    <t>Pictures of the second peripheral cutting edge</t>
   </si>
 </sst>
 </file>
@@ -1108,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CAD10C-4E89-4AC8-9C59-7B36AAFDF76D}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1468,10 +1469,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>82</v>
@@ -1485,7 +1486,7 @@
         <v>144</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>83</v>
@@ -1502,7 +1503,7 @@
         <v>145</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>83</v>
@@ -1516,10 +1517,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>83</v>
@@ -1533,10 +1534,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>83</v>
@@ -1550,10 +1551,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>82</v>
@@ -1648,10 +1649,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>116</v>
@@ -1662,10 +1663,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>116</v>
@@ -1896,7 +1897,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1963,18 +1964,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2160,7 +2161,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2475,7 +2476,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A5" sqref="A5:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2484,7 +2485,7 @@
     <col min="2" max="2" width="13.3046875" customWidth="1"/>
     <col min="3" max="3" width="12.07421875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
@@ -2531,7 +2532,7 @@
         <v>121</v>
       </c>
       <c r="D5" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>133</v>
@@ -2547,9 +2548,6 @@
       <c r="C6" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D6" s="9">
-        <v>1</v>
-      </c>
       <c r="E6" s="9" t="s">
         <v>136</v>
       </c>
@@ -2579,10 +2577,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
@@ -2593,38 +2591,38 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E9" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
         <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E11" t="s">
         <v>166</v>
@@ -2632,61 +2630,61 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="D14" t="s">
         <v>137</v>
       </c>
       <c r="E14" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="E15" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
@@ -2788,8 +2786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB419CFD-8D63-4604-B9FB-5116F92A3DFA}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2805,7 +2803,7 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -2813,7 +2811,7 @@
         <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -3103,8 +3101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A181C8CB-755B-4719-BE72-E29AF133B308}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3121,7 +3119,7 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -3129,7 +3127,7 @@
         <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -3160,7 +3158,7 @@
         <v>121</v>
       </c>
       <c r="D5" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>133</v>
@@ -3176,9 +3174,6 @@
       <c r="C6" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D6" s="9">
-        <v>1</v>
-      </c>
       <c r="E6" s="9" t="s">
         <v>136</v>
       </c>
@@ -3208,10 +3203,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
@@ -3222,38 +3217,38 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E9" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
         <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E11" t="s">
         <v>166</v>
@@ -3261,61 +3256,61 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="D14" t="s">
         <v>137</v>
       </c>
       <c r="E14" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="E15" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Removed "experiment" from twm profiles
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48387402-4FAA-46A8-8AD8-687B4F02661E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FE7C0C-1A72-4BD4-B462-4A995CC4A65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="7" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="4" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="171">
   <si>
     <t>Person</t>
   </si>
@@ -2158,10 +2158,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32959709-6667-403C-8910-69C88EF04E98}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2249,38 +2249,41 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
         <v>69</v>
       </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>108</v>
+        <v>25</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="5" t="s">
-        <v>38</v>
+      <c r="A10" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>123</v>
@@ -2288,16 +2291,13 @@
       <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" t="s">
-        <v>99</v>
+      <c r="D10">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>123</v>
@@ -2306,12 +2306,12 @@
         <v>25</v>
       </c>
       <c r="D11">
-        <v>80</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>123</v>
@@ -2320,12 +2320,12 @@
         <v>25</v>
       </c>
       <c r="D12">
-        <v>0.05</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>123</v>
@@ -2334,12 +2334,12 @@
         <v>25</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -2348,12 +2348,12 @@
         <v>25</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>123</v>
@@ -2362,12 +2362,12 @@
         <v>25</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>123</v>
@@ -2375,13 +2375,13 @@
       <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="D16">
-        <v>2</v>
+      <c r="D16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>123</v>
@@ -2390,26 +2390,26 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
+        <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>2</v>
@@ -2418,20 +2418,6 @@
         <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2445,25 +2431,25 @@
           <x14:formula1>
             <xm:f>lists!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>B44:B224</xm:sqref>
+          <xm:sqref>B43:B223</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B7A0B58-18CB-4E89-A00B-6A6CC4604B9A}">
           <x14:formula1>
             <xm:f>categories!$A$2:$A$47</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C219</xm:sqref>
+          <xm:sqref>C5:C218</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EF44D3A9-49EA-4D01-9F82-1BAE12FAAAF2}">
           <x14:formula1>
             <xm:f>fields!$A$2:$A$259</xm:f>
           </x14:formula1>
-          <xm:sqref>A5:A267</xm:sqref>
+          <xm:sqref>A5:A266</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FEC87DC-4E62-4524-8120-5BAF6E7A2550}">
           <x14:formula1>
             <xm:f>lists!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B43</xm:sqref>
+          <xm:sqref>B5:B42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2476,7 +2462,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E16"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2784,10 +2770,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB419CFD-8D63-4604-B9FB-5116F92A3DFA}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2875,38 +2861,41 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
         <v>69</v>
       </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>108</v>
+        <v>25</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="5" t="s">
-        <v>38</v>
+      <c r="A10" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>123</v>
@@ -2914,16 +2903,13 @@
       <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" t="s">
-        <v>99</v>
+      <c r="D10">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>123</v>
@@ -2932,12 +2918,12 @@
         <v>25</v>
       </c>
       <c r="D11">
-        <v>80</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>123</v>
@@ -2946,12 +2932,12 @@
         <v>25</v>
       </c>
       <c r="D12">
-        <v>0.05</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>123</v>
@@ -2960,12 +2946,12 @@
         <v>25</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -2979,7 +2965,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>123</v>
@@ -2988,12 +2974,12 @@
         <v>25</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>123</v>
@@ -3001,13 +2987,13 @@
       <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="D16">
-        <v>2</v>
+      <c r="D16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>123</v>
@@ -3016,26 +3002,26 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>123</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
+        <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>2</v>
@@ -3044,20 +3030,6 @@
         <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3067,29 +3039,29 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACBF88F1-C2B2-4229-AE02-DC1813692D26}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B43:B223</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A0143D08-078D-4597-8514-5B4F5F9A50FB}">
           <x14:formula1>
             <xm:f>lists!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B43</xm:sqref>
+          <xm:sqref>B5:B42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE3391A2-FF63-4508-8FED-6B395E046851}">
           <x14:formula1>
             <xm:f>fields!$A$2:$A$259</xm:f>
           </x14:formula1>
-          <xm:sqref>A5:A267</xm:sqref>
+          <xm:sqref>A5:A266</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{779DB705-5571-4E35-BC3A-257148DC9F82}">
           <x14:formula1>
             <xm:f>categories!$A$2:$A$47</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C219</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACBF88F1-C2B2-4229-AE02-DC1813692D26}">
-          <x14:formula1>
-            <xm:f>lists!$A$2:$A$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>B44:B224</xm:sqref>
+          <xm:sqref>C5:C218</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3101,7 +3073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A181C8CB-755B-4719-BE72-E29AF133B308}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed asterisk for requried meta
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FE7C0C-1A72-4BD4-B462-4A995CC4A65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C151A1-54C5-4C2F-A793-7A4674FF23FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="4" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="174">
   <si>
     <t>Person</t>
   </si>
@@ -641,6 +641,15 @@
   </si>
   <si>
     <t>Pictures of the second peripheral cutting edge</t>
+  </si>
+  <si>
+    <t>Person responsible for conducting the measurement.</t>
+  </si>
+  <si>
+    <t>CIRP institution at which the measurement is captured.</t>
+  </si>
+  <si>
+    <t>Machine tool in which the measurement was conducted.</t>
   </si>
 </sst>
 </file>
@@ -2161,7 +2170,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2216,7 +2225,7 @@
         <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -2230,7 +2239,7 @@
         <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -2244,7 +2253,7 @@
         <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
@@ -2260,9 +2269,6 @@
       <c r="D8" t="s">
         <v>108</v>
       </c>
-      <c r="E8" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2277,9 +2283,6 @@
       <c r="D9" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="E9" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
@@ -2379,7 +2382,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -2403,11 +2406,8 @@
       <c r="C18" t="s">
         <v>71</v>
       </c>
-      <c r="E18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -2416,9 +2416,6 @@
       </c>
       <c r="C19" t="s">
         <v>71</v>
-      </c>
-      <c r="E19" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2773,13 +2770,13 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="21.4609375" customWidth="1"/>
-    <col min="2" max="2" width="19.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.4609375" customWidth="1"/>
     <col min="4" max="4" width="11.84375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
   </cols>
@@ -2828,7 +2825,7 @@
         <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -2842,7 +2839,7 @@
         <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -2856,7 +2853,7 @@
         <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
@@ -2872,9 +2869,6 @@
       <c r="D8" t="s">
         <v>108</v>
       </c>
-      <c r="E8" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
@@ -2889,9 +2883,6 @@
       <c r="D9" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="E9" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
@@ -2991,7 +2982,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
@@ -3005,7 +2996,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -3015,11 +3006,8 @@
       <c r="C18" t="s">
         <v>71</v>
       </c>
-      <c r="E18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -3028,9 +3016,6 @@
       </c>
       <c r="C19" t="s">
         <v>71</v>
-      </c>
-      <c r="E19" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed tool D to R
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D665C9DB-9F10-4AB4-899E-945C3B82589E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE284AF-A497-4B6A-9AAF-481F3EB9AE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="7" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="6" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -612,48 +612,6 @@
     <t>Overall Tool Wear</t>
   </si>
   <si>
-    <t>tool_d_at_0</t>
-  </si>
-  <si>
-    <t>tool_d_at_1</t>
-  </si>
-  <si>
-    <t>tool_d_at_2</t>
-  </si>
-  <si>
-    <t>tool_d_at_3</t>
-  </si>
-  <si>
-    <t>tool_d_at_4</t>
-  </si>
-  <si>
-    <t>tool_d_at_5</t>
-  </si>
-  <si>
-    <t>tool_d_at_6</t>
-  </si>
-  <si>
-    <t>Tool Diameter at 1mm</t>
-  </si>
-  <si>
-    <t>Tool Diameter at 2mm</t>
-  </si>
-  <si>
-    <t>Tool Diameter at 3mm</t>
-  </si>
-  <si>
-    <t>Tool Diameter at 4mm</t>
-  </si>
-  <si>
-    <t>Tool Diameter at 5mm</t>
-  </si>
-  <si>
-    <t>Tool Diameter at 6mm</t>
-  </si>
-  <si>
-    <t>Tool Diameter at 0mm</t>
-  </si>
-  <si>
     <t>first_peripheral_pictures</t>
   </si>
   <si>
@@ -675,27 +633,6 @@
     <t>abnormal_tool_wear</t>
   </si>
   <si>
-    <t>Tool diameter at a height of 1mm from the face</t>
-  </si>
-  <si>
-    <t>Tool diameter at a height of 2mm from the face</t>
-  </si>
-  <si>
-    <t>Tool diameter at a height of 3mm from the face</t>
-  </si>
-  <si>
-    <t>Tool diameter at a height of 4mm from the face</t>
-  </si>
-  <si>
-    <t>Tool diameter at a height of 5mm from the face</t>
-  </si>
-  <si>
-    <t>Tool diameter at a height of 6mm from the face (reference - not in cut)</t>
-  </si>
-  <si>
-    <t>Tool diameter at a height of 0mm from the face (at the cutter's face)</t>
-  </si>
-  <si>
     <t>Picture of the first cutting edge (peripheral)</t>
   </si>
   <si>
@@ -790,6 +727,69 @@
   </si>
   <si>
     <t>Signs of abnormal wear (buildup, chipping) in this run - Comment!</t>
+  </si>
+  <si>
+    <t>tool_r_at_0</t>
+  </si>
+  <si>
+    <t>tool_r_at_1</t>
+  </si>
+  <si>
+    <t>tool_r_at_2</t>
+  </si>
+  <si>
+    <t>tool_r_at_3</t>
+  </si>
+  <si>
+    <t>tool_r_at_4</t>
+  </si>
+  <si>
+    <t>tool_r_at_5</t>
+  </si>
+  <si>
+    <t>tool_r_at_6</t>
+  </si>
+  <si>
+    <t>Tool Radius at 0mm</t>
+  </si>
+  <si>
+    <t>Tool Radius at 1mm</t>
+  </si>
+  <si>
+    <t>Tool Radius at 2mm</t>
+  </si>
+  <si>
+    <t>Tool Radius at 3mm</t>
+  </si>
+  <si>
+    <t>Tool Radius at 4mm</t>
+  </si>
+  <si>
+    <t>Tool Radius at 5mm</t>
+  </si>
+  <si>
+    <t>Tool Radius at 6mm</t>
+  </si>
+  <si>
+    <t>Tool radius at a height of 0mm from the face (at the cutter's face)</t>
+  </si>
+  <si>
+    <t>Tool radius at a height of 1mm from the face</t>
+  </si>
+  <si>
+    <t>Tool radius at a height of 2mm from the face</t>
+  </si>
+  <si>
+    <t>Tool radius at a height of 3mm from the face</t>
+  </si>
+  <si>
+    <t>Tool radius at a height of 4mm from the face</t>
+  </si>
+  <si>
+    <t>Tool radius at a height of 5mm from the face</t>
+  </si>
+  <si>
+    <t>Tool radius at a height of 6mm from the face (reference - not in cut)</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1265,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1613,7 +1613,7 @@
         <v>132</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>80</v>
@@ -1779,7 +1779,7 @@
         <v>129</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>84</v>
@@ -1793,7 +1793,7 @@
         <v>130</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>84</v>
@@ -1832,10 +1832,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>81</v>
@@ -1849,10 +1849,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>168</v>
+        <v>208</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>81</v>
@@ -1866,10 +1866,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>81</v>
@@ -1883,10 +1883,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>81</v>
@@ -1900,10 +1900,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>171</v>
+        <v>211</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>81</v>
@@ -1917,10 +1917,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>172</v>
+        <v>212</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>81</v>
@@ -1934,10 +1934,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>81</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>143</v>
@@ -1965,10 +1965,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>114</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>151</v>
@@ -1993,10 +1993,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>114</v>
@@ -2007,10 +2007,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>80</v>
@@ -2386,7 +2386,7 @@
         <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -2409,7 +2409,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="D3" t="s">
         <v>78</v>
@@ -2432,7 +2432,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
         <v>39</v>
@@ -2449,7 +2449,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="E5" t="s">
         <v>41</v>
@@ -2463,7 +2463,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -2474,7 +2474,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="F7" t="s">
         <v>111</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="F8" t="s">
         <v>112</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="F9" t="s">
         <v>113</v>
@@ -2498,57 +2498,57 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C11" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C16" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C19" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C20" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.4">
@@ -2893,7 +2893,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2949,7 +2949,7 @@
         <v>119</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
@@ -2963,7 +2963,7 @@
         <v>119</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -2980,12 +2980,12 @@
         <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -2997,12 +2997,12 @@
         <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -3011,12 +3011,12 @@
         <v>159</v>
       </c>
       <c r="E9" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -3025,12 +3025,12 @@
         <v>159</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
@@ -3039,12 +3039,12 @@
         <v>159</v>
       </c>
       <c r="E11" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -3053,12 +3053,12 @@
         <v>159</v>
       </c>
       <c r="E12" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
@@ -3067,12 +3067,12 @@
         <v>159</v>
       </c>
       <c r="E13" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
@@ -3081,12 +3081,12 @@
         <v>159</v>
       </c>
       <c r="E14" t="s">
-        <v>186</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
@@ -3095,12 +3095,12 @@
         <v>159</v>
       </c>
       <c r="E15" t="s">
-        <v>187</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
@@ -3109,12 +3109,12 @@
         <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
@@ -3123,12 +3123,12 @@
         <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
@@ -3137,12 +3137,12 @@
         <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
@@ -3151,7 +3151,7 @@
         <v>153</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
@@ -3165,7 +3165,7 @@
         <v>117</v>
       </c>
       <c r="E20" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -3241,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB419CFD-8D63-4604-B9FB-5116F92A3DFA}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3544,7 +3544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A181C8CB-755B-4719-BE72-E29AF133B308}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -3601,7 +3601,7 @@
         <v>119</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
@@ -3615,7 +3615,7 @@
         <v>119</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -3632,12 +3632,12 @@
         <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -3649,12 +3649,12 @@
         <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -3663,12 +3663,12 @@
         <v>159</v>
       </c>
       <c r="E9" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -3677,12 +3677,12 @@
         <v>159</v>
       </c>
       <c r="E10" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
@@ -3691,12 +3691,12 @@
         <v>159</v>
       </c>
       <c r="E11" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -3705,12 +3705,12 @@
         <v>159</v>
       </c>
       <c r="E12" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
@@ -3719,12 +3719,12 @@
         <v>159</v>
       </c>
       <c r="E13" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
@@ -3733,12 +3733,12 @@
         <v>159</v>
       </c>
       <c r="E14" t="s">
-        <v>186</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
@@ -3747,12 +3747,12 @@
         <v>159</v>
       </c>
       <c r="E15" t="s">
-        <v>187</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
@@ -3761,12 +3761,12 @@
         <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
@@ -3775,12 +3775,12 @@
         <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
@@ -3789,12 +3789,12 @@
         <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
@@ -3803,7 +3803,7 @@
         <v>153</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
@@ -3817,7 +3817,7 @@
         <v>117</v>
       </c>
       <c r="E20" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Metadata Rework: No more typescript types parsed
The idea until now was to parse the metadata.xlsx into a .yaml file for
loading the data and into a d.ts file to create type-safety when
building the components for it.

This is however an approach that mixes data and data structure.

We now only parse the metadata.xlsx into a yaml file for the data and
have a fixed types file on hand. The structure of how a parameter and a
profile are defined will not change unless we change the system, so the
types that go along it are not required to be code-generated.

This is the first step in removing the metadata responsibility from the
client. We want to shift it to ICOapi to use interchangeable files, and
the client can't easily access the filesystem.
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465E3C90-BEA4-48A7-AA40-6CBEF9AAFB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFD4713-A6C8-4668-B239-2D9BBE638387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="7" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="6" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -3442,8 +3445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB419CFD-8D63-4604-B9FB-5116F92A3DFA}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3765,7 +3768,7 @@
         <v>25</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
@@ -3858,7 +3861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A181C8CB-755B-4719-BE72-E29AF133B308}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Metadata Rework: Make Input Types Explicit
This reworks the core MetaInput.vue to use explicit components based on
the input's datatype and not the <component :is=""> syntax.
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFD4713-A6C8-4668-B239-2D9BBE638387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59C50DE-73A1-4AF4-B536-45496DD14067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="6" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="321">
   <si>
     <t>Person</t>
   </si>
@@ -375,9 +375,6 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>float</t>
-  </si>
-  <si>
     <t>twm_layer</t>
   </si>
   <si>
@@ -474,9 +471,6 @@
     <t>Thread Milling</t>
   </si>
   <si>
-    <t>file</t>
-  </si>
-  <si>
     <t>files</t>
   </si>
   <si>
@@ -781,9 +775,6 @@
   </si>
   <si>
     <t>tool_id</t>
-  </si>
-  <si>
-    <t>Tool ID</t>
   </si>
   <si>
     <t>Tool radius at the tip before any cut (initial inspection)</t>
@@ -836,6 +827,273 @@
   </si>
   <si>
     <t>cirp_twm_2</t>
+  </si>
+  <si>
+    <t>setup_pictures</t>
+  </si>
+  <si>
+    <t>Pictures of Complete Setup</t>
+  </si>
+  <si>
+    <t>Pictures of the complete setup in the machine for future reference.</t>
+  </si>
+  <si>
+    <t>machine_manufacturer</t>
+  </si>
+  <si>
+    <t>Manufacturer of Machine Tool</t>
+  </si>
+  <si>
+    <t>machine_model</t>
+  </si>
+  <si>
+    <t>Model of Machine Tool</t>
+  </si>
+  <si>
+    <t>machine_serial</t>
+  </si>
+  <si>
+    <t>Serial Number of Machine Tool</t>
+  </si>
+  <si>
+    <t>machine_travel_x</t>
+  </si>
+  <si>
+    <t>Machine Travel Range (X)</t>
+  </si>
+  <si>
+    <t>machine_travel_y</t>
+  </si>
+  <si>
+    <t>machine_travel_z</t>
+  </si>
+  <si>
+    <t>Machine Travel Range (Y)</t>
+  </si>
+  <si>
+    <t>Machine Travel Range (Z)</t>
+  </si>
+  <si>
+    <t>machine_has_axis_a</t>
+  </si>
+  <si>
+    <t>machine_has_axis_c</t>
+  </si>
+  <si>
+    <t>Machine has A Axis</t>
+  </si>
+  <si>
+    <t>Machine has C Axis</t>
+  </si>
+  <si>
+    <t>Max. Spindle Speed</t>
+  </si>
+  <si>
+    <t>machine_spindle_max_speed</t>
+  </si>
+  <si>
+    <t>machine_spindle_max_torque</t>
+  </si>
+  <si>
+    <t>Max. Spindle Torque</t>
+  </si>
+  <si>
+    <t>machine_spindle_max_power</t>
+  </si>
+  <si>
+    <t>Max. Spindle Power</t>
+  </si>
+  <si>
+    <t>Exact model or model number of the machine tool.</t>
+  </si>
+  <si>
+    <t>Manufacturer of the machine tool.</t>
+  </si>
+  <si>
+    <t>Serial number of the machine tool for identification.</t>
+  </si>
+  <si>
+    <t>Travel range of the machine tool in the X direction.</t>
+  </si>
+  <si>
+    <t>Travel range of the machine tool in the Y direction.</t>
+  </si>
+  <si>
+    <t>Travel range of the machine tool in the Z direction.</t>
+  </si>
+  <si>
+    <t>Check if the machine tool has an A axis.</t>
+  </si>
+  <si>
+    <t>Check if the machine tool has a C axis.</t>
+  </si>
+  <si>
+    <t>The maximum spindle speed of the machine tool.</t>
+  </si>
+  <si>
+    <t>The maximum spindle torque of the machine tool.</t>
+  </si>
+  <si>
+    <t>The maximum spindle power of the machine tool.</t>
+  </si>
+  <si>
+    <t>tool</t>
+  </si>
+  <si>
+    <t>Tool Definition</t>
+  </si>
+  <si>
+    <t>tool_stickout</t>
+  </si>
+  <si>
+    <t>Tool Stickout from Collet</t>
+  </si>
+  <si>
+    <t>tool_type</t>
+  </si>
+  <si>
+    <t>Tool Type</t>
+  </si>
+  <si>
+    <t>tool_manufacturer</t>
+  </si>
+  <si>
+    <t>Tool Manufacturer</t>
+  </si>
+  <si>
+    <t>tool_nominal_diameter</t>
+  </si>
+  <si>
+    <t>Nominal Tool Diameter</t>
+  </si>
+  <si>
+    <t>Stickout length of the tool measured from the collet nut.</t>
+  </si>
+  <si>
+    <t>Manufacturer's tool type identification (e.g. article number, code, …)</t>
+  </si>
+  <si>
+    <t>Manufacturer of the tool.</t>
+  </si>
+  <si>
+    <t>Nominal Diameter of the tool.</t>
+  </si>
+  <si>
+    <t>botek</t>
+  </si>
+  <si>
+    <t>Manufacturer specification of tool material.</t>
+  </si>
+  <si>
+    <t>Tool tooth count.</t>
+  </si>
+  <si>
+    <t>workpiece</t>
+  </si>
+  <si>
+    <t>Workpiece Definition</t>
+  </si>
+  <si>
+    <t>Machine Tool Definition</t>
+  </si>
+  <si>
+    <t>workpiece_id</t>
+  </si>
+  <si>
+    <t>Workpiece Identification</t>
+  </si>
+  <si>
+    <t>Tool Identification</t>
+  </si>
+  <si>
+    <t>workpiece_length</t>
+  </si>
+  <si>
+    <t>workpiece_height</t>
+  </si>
+  <si>
+    <t>workpiece_width</t>
+  </si>
+  <si>
+    <t>Workpiece Length</t>
+  </si>
+  <si>
+    <t>Workpiece Height</t>
+  </si>
+  <si>
+    <t>Workpiece Width</t>
+  </si>
+  <si>
+    <t>workpiece_temper</t>
+  </si>
+  <si>
+    <t>Workpiece Thermal Treatment</t>
+  </si>
+  <si>
+    <t>TSC</t>
+  </si>
+  <si>
+    <t>TSC+Flood</t>
+  </si>
+  <si>
+    <t>Annealed</t>
+  </si>
+  <si>
+    <t>Hardened + Tempered</t>
+  </si>
+  <si>
+    <t>Hardened (w.o. tempering)</t>
+  </si>
+  <si>
+    <t>Stress Relieved</t>
+  </si>
+  <si>
+    <t>Identification number / code of the specific workpiece.</t>
+  </si>
+  <si>
+    <t>Length of the workpiece (longest side)</t>
+  </si>
+  <si>
+    <t>Height of the workpiece</t>
+  </si>
+  <si>
+    <t>Width of the Workpiece</t>
+  </si>
+  <si>
+    <t>Material code / name of the workpiece</t>
+  </si>
+  <si>
+    <t>Tempering state of the workpiece</t>
+  </si>
+  <si>
+    <t>workpiece_hardness</t>
+  </si>
+  <si>
+    <t>Workpiece Hardness</t>
+  </si>
+  <si>
+    <t>HRC</t>
+  </si>
+  <si>
+    <t>Hardness of the workpiece in HRC</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>Nm</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>float_qty</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
 </sst>
 </file>
@@ -898,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -912,11 +1170,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1311,10 +1628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CAD10C-4E89-4AC8-9C59-7B36AAFDF76D}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1436,8 +1753,8 @@
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>81</v>
+      <c r="C8" s="3" t="s">
+        <v>319</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>51</v>
@@ -1454,7 +1771,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>54</v>
@@ -1471,7 +1788,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>52</v>
@@ -1488,7 +1805,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>53</v>
@@ -1505,7 +1822,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>53</v>
@@ -1522,7 +1839,7 @@
         <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>53</v>
@@ -1539,7 +1856,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>53</v>
@@ -1556,7 +1873,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>53</v>
@@ -1573,7 +1890,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="3" t="s">
@@ -1603,7 +1920,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>53</v>
@@ -1639,7 +1956,7 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -1654,15 +1971,15 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>80</v>
@@ -1673,10 +1990,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>80</v>
@@ -1687,13 +2004,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>53</v>
@@ -1704,13 +2021,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>53</v>
@@ -1721,13 +2038,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>53</v>
@@ -1738,13 +2055,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>53</v>
@@ -1755,10 +2072,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>80</v>
@@ -1769,13 +2086,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>58</v>
@@ -1783,13 +2100,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>114</v>
+        <v>320</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>58</v>
@@ -1797,13 +2114,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>58</v>
@@ -1811,10 +2128,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>50</v>
@@ -1825,13 +2142,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>58</v>
@@ -1839,13 +2156,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>58</v>
@@ -1853,13 +2170,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>58</v>
@@ -1867,27 +2184,28 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>114</v>
-      </c>
+        <v>320</v>
+      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>114</v>
+        <v>320</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>58</v>
@@ -1895,13 +2213,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>53</v>
@@ -1912,13 +2230,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>53</v>
@@ -1929,13 +2247,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>53</v>
@@ -1946,13 +2264,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>53</v>
@@ -1963,13 +2281,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>53</v>
@@ -1980,13 +2298,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>53</v>
@@ -1997,13 +2315,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>81</v>
+        <v>319</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>53</v>
@@ -2014,13 +2332,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>114</v>
+        <v>320</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>58</v>
@@ -2028,13 +2346,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="C46" s="2" t="s">
-        <v>114</v>
+        <v>320</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>58</v>
@@ -2042,13 +2360,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>114</v>
+        <v>320</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>58</v>
@@ -2056,13 +2374,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="C48" s="2" t="s">
-        <v>114</v>
+        <v>320</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>58</v>
@@ -2070,10 +2388,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>80</v>
@@ -2084,10 +2402,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>217</v>
+        <v>290</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>49</v>
@@ -2096,54 +2414,431 @@
         <v>58</v>
       </c>
     </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A51" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A52" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A53" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A55" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A56" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A57" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A58" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A59" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A60" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A61" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A62" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A65" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A66" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C1:E24 C29:E34 C36:E1048576">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="suggestions">
+  <conditionalFormatting sqref="C1:E24 C29:E34 C36:E55 C58:E1048576">
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="suggestions">
       <formula>NOT(ISERROR(SEARCH("suggestions",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Dropdown">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="Dropdown">
       <formula>NOT(ISERROR(SEARCH("Dropdown",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:E35">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="suggestions">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="suggestions">
       <formula>NOT(ISERROR(SEARCH("suggestions",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Dropdown">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Dropdown">
       <formula>NOT(ISERROR(SEARCH("Dropdown",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:E25">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="suggestions">
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="suggestions">
       <formula>NOT(ISERROR(SEARCH("suggestions",C25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Dropdown">
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="Dropdown">
       <formula>NOT(ISERROR(SEARCH("Dropdown",C25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:E26">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="suggestions">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="suggestions">
       <formula>NOT(ISERROR(SEARCH("suggestions",C26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Dropdown">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="Dropdown">
       <formula>NOT(ISERROR(SEARCH("Dropdown",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:E27">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="suggestions">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="suggestions">
       <formula>NOT(ISERROR(SEARCH("suggestions",C27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Dropdown">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Dropdown">
       <formula>NOT(ISERROR(SEARCH("Dropdown",C27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:E28">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="suggestions">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="suggestions">
       <formula>NOT(ISERROR(SEARCH("suggestions",C28)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Dropdown">
+      <formula>NOT(ISERROR(SEARCH("Dropdown",C28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57:E57">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="suggestions">
+      <formula>NOT(ISERROR(SEARCH("suggestions",D57)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Dropdown">
+      <formula>NOT(ISERROR(SEARCH("Dropdown",D57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56:E56">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="suggestions">
+      <formula>NOT(ISERROR(SEARCH("suggestions",D56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Dropdown">
+      <formula>NOT(ISERROR(SEARCH("Dropdown",D56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="suggestions">
+      <formula>NOT(ISERROR(SEARCH("suggestions",C56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Dropdown">
+      <formula>NOT(ISERROR(SEARCH("Dropdown",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="suggestions">
+      <formula>NOT(ISERROR(SEARCH("suggestions",C57)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Dropdown">
-      <formula>NOT(ISERROR(SEARCH("Dropdown",C28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Dropdown",C57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2180,7 +2875,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -2188,7 +2883,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>76</v>
@@ -2197,7 +2892,7 @@
         <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
@@ -2208,23 +2903,23 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -2316,16 +3011,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5990D1-DFF5-4992-8B2C-80C0C460D997}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
@@ -2362,58 +3057,82 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
         <v>149</v>
-      </c>
-      <c r="B8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" t="s">
         <v>150</v>
-      </c>
-      <c r="B9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>268</v>
+      </c>
+      <c r="B13" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>285</v>
+      </c>
+      <c r="B14" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2424,23 +3143,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D57FB1A-6D98-4995-87AD-13E81E29DC39}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="12.53515625" customWidth="1"/>
     <col min="3" max="3" width="31.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.3046875" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.07421875" customWidth="1"/>
     <col min="6" max="6" width="24.69140625" customWidth="1"/>
     <col min="7" max="7" width="17.84375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -2450,7 +3170,7 @@
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -2460,10 +3180,13 @@
         <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+        <v>121</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2471,22 +3194,25 @@
         <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
+        <v>165</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2494,22 +3220,25 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
+        <v>166</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="E3" t="s">
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+        <v>124</v>
+      </c>
+      <c r="H3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2517,123 +3246,138 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>167</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
         <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+        <v>108</v>
+      </c>
+      <c r="H5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
       </c>
       <c r="F6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C9" t="s">
         <v>172</v>
       </c>
-      <c r="F7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C8" t="s">
+      <c r="F9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C10" t="s">
         <v>173</v>
       </c>
-      <c r="F8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C9" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C11" t="s">
         <v>174</v>
       </c>
-      <c r="F9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C10" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C12" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C11" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C13" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C12" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C13" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C14" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C16" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="C16" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.4">
@@ -2641,6 +3385,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2659,7 +3404,7 @@
         <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -2672,15 +3417,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32959709-6667-403C-8910-69C88EF04E98}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.4609375" customWidth="1"/>
+    <col min="1" max="1" width="25.921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.3046875" customWidth="1"/>
     <col min="3" max="3" width="14.921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.84375" bestFit="1" customWidth="1"/>
@@ -2692,7 +3437,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -2700,7 +3445,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -2708,7 +3453,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>76</v>
@@ -2717,7 +3462,7 @@
         <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
@@ -2731,7 +3476,7 @@
         <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -2745,313 +3490,629 @@
         <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>268</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" t="s">
+        <v>268</v>
+      </c>
+      <c r="D20" s="2">
+        <v>35</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" t="s">
+        <v>268</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" t="s">
+        <v>268</v>
+      </c>
+      <c r="D23" s="2">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" t="s">
+        <v>268</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" t="s">
+        <v>268</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>212</v>
+      </c>
+      <c r="E26" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>212</v>
+      </c>
+      <c r="E27" t="s">
         <v>216</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>214</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>212</v>
+      </c>
+      <c r="E28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>212</v>
+      </c>
+      <c r="E29" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E10" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>212</v>
+      </c>
+      <c r="E30" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>214</v>
-      </c>
-      <c r="E11" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>212</v>
+      </c>
+      <c r="E31" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>214</v>
-      </c>
-      <c r="E12" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>212</v>
+      </c>
+      <c r="E32" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>214</v>
-      </c>
-      <c r="E13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>214</v>
-      </c>
-      <c r="E14" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>214</v>
-      </c>
-      <c r="E15" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" s="5" t="s">
+    <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D34" s="2">
+        <v>200</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D35" s="2">
+        <v>100</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D36" s="2">
+        <v>100</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B40" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B46" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
         <v>25</v>
       </c>
-      <c r="D16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" s="2" t="s">
+      <c r="D46" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B47" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B29" s="5"/>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B49" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3063,25 +4124,25 @@
           <x14:formula1>
             <xm:f>lists!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>B45:B225</xm:sqref>
+          <xm:sqref>B65:B245</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B7A0B58-18CB-4E89-A00B-6A6CC4604B9A}">
           <x14:formula1>
             <xm:f>categories!$A$2:$A$47</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C7 C8:C220</xm:sqref>
+          <xm:sqref>C5:C240</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EF44D3A9-49EA-4D01-9F82-1BAE12FAAAF2}">
           <x14:formula1>
             <xm:f>fields!$A$2:$A$260</xm:f>
           </x14:formula1>
-          <xm:sqref>A5:A7 A8:A268</xm:sqref>
+          <xm:sqref>A5:A288</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FEC87DC-4E62-4524-8120-5BAF6E7A2550}">
           <x14:formula1>
             <xm:f>lists!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B7 B8:B44</xm:sqref>
+          <xm:sqref>B5:B64</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3094,7 +4155,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3111,7 +4172,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -3119,7 +4180,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -3127,7 +4188,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>76</v>
@@ -3136,240 +4197,252 @@
         <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D5" s="9">
         <v>8</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="D16" t="s">
+        <v>318</v>
       </c>
       <c r="E16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="D17" t="s">
+        <v>318</v>
       </c>
       <c r="E17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="D18" t="s">
+        <v>318</v>
       </c>
       <c r="E18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="D19" t="s">
+        <v>318</v>
       </c>
       <c r="E19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -3445,8 +4518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB419CFD-8D63-4604-B9FB-5116F92A3DFA}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3463,7 +4536,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -3471,7 +4544,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -3479,7 +4552,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>76</v>
@@ -3488,7 +4561,7 @@
         <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
@@ -3502,7 +4575,7 @@
         <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -3516,7 +4589,7 @@
         <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -3530,12 +4603,12 @@
         <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -3544,105 +4617,105 @@
         <v>67</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E11" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E12" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E13" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
@@ -3650,13 +4723,13 @@
         <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
@@ -3664,7 +4737,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
@@ -3678,7 +4751,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -3692,7 +4765,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -3706,13 +4779,13 @@
         <v>37</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
@@ -3720,7 +4793,7 @@
         <v>27</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
@@ -3734,7 +4807,7 @@
         <v>44</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -3748,7 +4821,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
@@ -3762,7 +4835,7 @@
         <v>32</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C24" t="s">
         <v>25</v>
@@ -3776,7 +4849,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
         <v>25</v>
@@ -3787,16 +4860,16 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
@@ -3879,7 +4952,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -3887,7 +4960,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -3895,7 +4968,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>76</v>
@@ -3904,240 +4977,240 @@
         <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D5" s="9">
         <v>8</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -4237,7 +5310,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -4245,7 +5318,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>76</v>
@@ -4254,7 +5327,7 @@
         <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
@@ -4268,7 +5341,7 @@
         <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -4282,7 +5355,7 @@
         <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -4296,7 +5369,7 @@
         <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
@@ -4310,7 +5383,7 @@
         <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
@@ -4324,10 +5397,10 @@
         <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
@@ -4341,7 +5414,7 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
@@ -4432,7 +5505,7 @@
         <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
@@ -4448,7 +5521,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
@@ -4468,7 +5541,7 @@
         <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
@@ -4482,7 +5555,7 @@
         <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Metadata Rework: Update metadata files
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59C50DE-73A1-4AF4-B536-45496DD14067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1648015F-BB4C-46A9-91F0-D846958B6B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="4" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="321">
   <si>
     <t>Person</t>
   </si>
@@ -1087,13 +1087,13 @@
     <t>kW</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>float_qty</t>
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>bokte_01</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +1630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CAD10C-4E89-4AC8-9C59-7B36AAFDF76D}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
@@ -1754,7 +1754,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>51</v>
@@ -1771,7 +1771,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>54</v>
@@ -1788,7 +1788,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>52</v>
@@ -1805,7 +1805,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>53</v>
@@ -1822,7 +1822,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>53</v>
@@ -1839,7 +1839,7 @@
         <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>53</v>
@@ -1856,7 +1856,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>53</v>
@@ -1873,7 +1873,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>53</v>
@@ -1920,7 +1920,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>53</v>
@@ -2010,7 +2010,7 @@
         <v>136</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>53</v>
@@ -2027,7 +2027,7 @@
         <v>137</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>53</v>
@@ -2044,7 +2044,7 @@
         <v>143</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>53</v>
@@ -2061,7 +2061,7 @@
         <v>144</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>53</v>
@@ -2106,7 +2106,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>58</v>
@@ -2190,7 +2190,7 @@
         <v>138</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="3" t="s">
@@ -2205,7 +2205,7 @@
         <v>146</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>58</v>
@@ -2219,7 +2219,7 @@
         <v>192</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>53</v>
@@ -2236,7 +2236,7 @@
         <v>193</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>53</v>
@@ -2253,7 +2253,7 @@
         <v>194</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>53</v>
@@ -2270,7 +2270,7 @@
         <v>195</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>53</v>
@@ -2287,7 +2287,7 @@
         <v>196</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>53</v>
@@ -2304,7 +2304,7 @@
         <v>197</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>53</v>
@@ -2321,7 +2321,7 @@
         <v>198</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>53</v>
@@ -2338,7 +2338,7 @@
         <v>138</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>58</v>
@@ -2352,7 +2352,7 @@
         <v>201</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>58</v>
@@ -2366,7 +2366,7 @@
         <v>146</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>58</v>
@@ -2380,7 +2380,7 @@
         <v>202</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>58</v>
@@ -2422,7 +2422,7 @@
         <v>233</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>58</v>
@@ -2478,7 +2478,7 @@
         <v>242</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>53</v>
@@ -2495,7 +2495,7 @@
         <v>245</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>53</v>
@@ -2512,7 +2512,7 @@
         <v>246</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>53</v>
@@ -2557,7 +2557,7 @@
         <v>251</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>315</v>
@@ -2574,7 +2574,7 @@
         <v>254</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>316</v>
@@ -2591,7 +2591,7 @@
         <v>256</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>317</v>
@@ -2608,7 +2608,7 @@
         <v>271</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>53</v>
@@ -2653,7 +2653,7 @@
         <v>277</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>53</v>
@@ -2684,7 +2684,7 @@
         <v>294</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>53</v>
@@ -2701,7 +2701,7 @@
         <v>295</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>53</v>
@@ -2718,7 +2718,7 @@
         <v>296</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>53</v>
@@ -2750,7 +2750,7 @@
         <v>312</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>313</v>
@@ -3419,8 +3419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32959709-6667-403C-8910-69C88EF04E98}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3707,6 +3707,9 @@
       </c>
       <c r="C21" t="s">
         <v>268</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>279</v>
@@ -4154,8 +4157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD63C287-BDD3-4AF4-BAC0-84A491537ABD}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4373,9 +4376,6 @@
       <c r="C16" t="s">
         <v>147</v>
       </c>
-      <c r="D16" t="s">
-        <v>318</v>
-      </c>
       <c r="E16" t="s">
         <v>159</v>
       </c>
@@ -4390,9 +4390,6 @@
       <c r="C17" t="s">
         <v>147</v>
       </c>
-      <c r="D17" t="s">
-        <v>318</v>
-      </c>
       <c r="E17" t="s">
         <v>210</v>
       </c>
@@ -4407,9 +4404,6 @@
       <c r="C18" t="s">
         <v>148</v>
       </c>
-      <c r="D18" t="s">
-        <v>318</v>
-      </c>
       <c r="E18" t="s">
         <v>160</v>
       </c>
@@ -4423,9 +4417,6 @@
       </c>
       <c r="C19" t="s">
         <v>148</v>
-      </c>
-      <c r="D19" t="s">
-        <v>318</v>
       </c>
       <c r="E19" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
Metadata Rework: Update profiles
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breurather\src\icoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1648015F-BB4C-46A9-91F0-D846958B6B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAD9C58-F8A4-47EC-BD6F-60EF20393886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="4" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="10" xr2:uid="{2B21317E-79C0-4BD6-8C8B-33401DD0D856}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,10 @@
     <sheet name="post_twm1" sheetId="7" r:id="rId6"/>
     <sheet name="pre_twm2" sheetId="10" r:id="rId7"/>
     <sheet name="post_twm2" sheetId="11" r:id="rId8"/>
-    <sheet name="pre_milling" sheetId="8" r:id="rId9"/>
-    <sheet name="post_milling" sheetId="9" r:id="rId10"/>
+    <sheet name="pre_twm_open" sheetId="12" r:id="rId9"/>
+    <sheet name="post_twm_open" sheetId="13" r:id="rId10"/>
+    <sheet name="pre_milling" sheetId="8" r:id="rId11"/>
+    <sheet name="post_milling" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -130,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="321">
   <si>
     <t>Person</t>
   </si>
@@ -519,9 +521,6 @@
     <t>tool_breakage</t>
   </si>
   <si>
-    <t>CIRP TWM 1 (ae=10mm)</t>
-  </si>
-  <si>
     <t>CIRP TWM 2 (ae=10mm)</t>
   </si>
   <si>
@@ -589,9 +588,6 @@
   </si>
   <si>
     <t>CIRP institution at which the measurement is captured.</t>
-  </si>
-  <si>
-    <t>Machine tool in which the measurement was conducted.</t>
   </si>
   <si>
     <t>wear</t>
@@ -1094,6 +1090,12 @@
   </si>
   <si>
     <t>bokte_01</t>
+  </si>
+  <si>
+    <t>cirp_twm_open</t>
+  </si>
+  <si>
+    <t>CIRP TWM OPEN</t>
   </si>
 </sst>
 </file>
@@ -1754,7 +1756,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>51</v>
@@ -1771,7 +1773,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>54</v>
@@ -1788,7 +1790,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>52</v>
@@ -1805,7 +1807,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>53</v>
@@ -1822,7 +1824,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>53</v>
@@ -1839,7 +1841,7 @@
         <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>53</v>
@@ -1856,7 +1858,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>53</v>
@@ -1873,7 +1875,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>53</v>
@@ -1920,7 +1922,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>53</v>
@@ -1979,7 +1981,7 @@
         <v>128</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>80</v>
@@ -1990,10 +1992,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>80</v>
@@ -2004,13 +2006,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>53</v>
@@ -2021,13 +2023,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>53</v>
@@ -2038,13 +2040,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>53</v>
@@ -2055,13 +2057,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>53</v>
@@ -2072,10 +2074,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>80</v>
@@ -2106,7 +2108,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>58</v>
@@ -2142,10 +2144,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>83</v>
@@ -2156,10 +2158,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>83</v>
@@ -2173,7 +2175,7 @@
         <v>126</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>83</v>
@@ -2184,13 +2186,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="3" t="s">
@@ -2199,13 +2201,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>58</v>
@@ -2213,13 +2215,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>53</v>
@@ -2230,13 +2232,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>53</v>
@@ -2247,13 +2249,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>53</v>
@@ -2264,13 +2266,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>53</v>
@@ -2281,13 +2283,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>53</v>
@@ -2298,13 +2300,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>53</v>
@@ -2315,13 +2317,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>53</v>
@@ -2332,13 +2334,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>58</v>
@@ -2346,13 +2348,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="C46" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>58</v>
@@ -2360,13 +2362,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>58</v>
@@ -2374,13 +2376,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="C48" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>58</v>
@@ -2388,10 +2390,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>80</v>
@@ -2402,10 +2404,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>49</v>
@@ -2416,13 +2418,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>58</v>
@@ -2430,10 +2432,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>49</v>
@@ -2444,10 +2446,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>49</v>
@@ -2458,10 +2460,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>49</v>
@@ -2472,13 +2474,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>53</v>
@@ -2489,13 +2491,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>245</v>
-      </c>
       <c r="C56" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>53</v>
@@ -2506,13 +2508,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="C57" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>53</v>
@@ -2523,10 +2525,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>80</v>
@@ -2537,10 +2539,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>80</v>
@@ -2551,16 +2553,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>58</v>
@@ -2568,16 +2570,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>58</v>
@@ -2585,16 +2587,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>58</v>
@@ -2602,13 +2604,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>53</v>
@@ -2619,10 +2621,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>49</v>
@@ -2633,10 +2635,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>49</v>
@@ -2647,13 +2649,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>53</v>
@@ -2664,10 +2666,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>49</v>
@@ -2678,13 +2680,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>53</v>
@@ -2695,13 +2697,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>53</v>
@@ -2712,13 +2714,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>53</v>
@@ -2729,10 +2731,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>55</v>
@@ -2744,16 +2746,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>58</v>
@@ -2848,6 +2850,676 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4403BA39-0A22-4007-B30D-BFD7F9F73D30}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="29.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3046875" customWidth="1"/>
+    <col min="3" max="3" width="12.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="9">
+        <v>6</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" s="2"/>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" s="2"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" s="2"/>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" s="2"/>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" s="2"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" s="2"/>
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="2"/>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" s="2"/>
+      <c r="B28" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86E24790-77C1-4852-B305-256079791FB6}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B42:B232</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47BBD5FA-BD80-4A0A-83B7-B5C5436E59CD}">
+          <x14:formula1>
+            <xm:f>fields!$A$2:$A$260</xm:f>
+          </x14:formula1>
+          <xm:sqref>A17:A275 A5:A15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E3C77AFE-A824-4823-8FC5-B5AABA3C3B68}">
+          <x14:formula1>
+            <xm:f>categories!$A$2:$A$47</xm:f>
+          </x14:formula1>
+          <xm:sqref>C17:C227 C5:C15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{65AE187B-699D-4225-A6ED-EC9A35D8D3C6}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:B41</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664D46D0-CFAB-416B-A253-FC2929E5C79F}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="21.4609375" customWidth="1"/>
+    <col min="2" max="2" width="13.3046875" customWidth="1"/>
+    <col min="4" max="4" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{592FF17C-EAEA-47DA-A2F3-BD8F9AEE7605}">
+          <x14:formula1>
+            <xm:f>fields!$A$2:$A$260</xm:f>
+          </x14:formula1>
+          <xm:sqref>A5:A269</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F7074770-80C9-43C1-B273-B5283AD6B093}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:B19 B21:B22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4A4167C6-AD91-46A4-A351-4832B091EE7E}">
+          <x14:formula1>
+            <xm:f>categories!$A$2:$A$47</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:C221</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{78A217F7-2DE2-45FF-81FF-3EEF5C9ED4C5}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B23:B226</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A08BA68E-8F08-43D8-B97F-D9845B5C1E39}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AABC585-1D59-4FE6-A0B8-95D5F4DF49F8}">
   <dimension ref="A1:E19"/>
   <sheetViews>
@@ -3081,34 +3753,34 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -3116,23 +3788,23 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -3183,7 +3855,7 @@
         <v>121</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
@@ -3194,7 +3866,7 @@
         <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>120</v>
@@ -3209,7 +3881,7 @@
         <v>123</v>
       </c>
       <c r="H2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
@@ -3220,7 +3892,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>63</v>
@@ -3235,7 +3907,7 @@
         <v>124</v>
       </c>
       <c r="H3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
@@ -3246,7 +3918,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>78</v>
@@ -3258,7 +3930,7 @@
         <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
@@ -3269,7 +3941,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E5" t="s">
         <v>41</v>
@@ -3278,7 +3950,7 @@
         <v>108</v>
       </c>
       <c r="H5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
@@ -3286,7 +3958,7 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -3297,10 +3969,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F7" t="s">
         <v>110</v>
@@ -3308,10 +3980,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F8" t="s">
         <v>111</v>
@@ -3319,7 +3991,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F9" t="s">
         <v>112</v>
@@ -3327,57 +3999,57 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.4">
@@ -3419,8 +4091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32959709-6667-403C-8910-69C88EF04E98}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3437,7 +4109,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -3476,7 +4148,7 @@
         <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -3490,12 +4162,12 @@
         <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -3504,12 +4176,12 @@
         <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -3518,12 +4190,12 @@
         <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
@@ -3532,12 +4204,12 @@
         <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -3546,12 +4218,12 @@
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
@@ -3560,12 +4232,12 @@
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
@@ -3574,12 +4246,12 @@
         <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
@@ -3588,12 +4260,12 @@
         <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
@@ -3605,12 +4277,12 @@
         <v>127</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
@@ -3622,12 +4294,12 @@
         <v>127</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
@@ -3636,12 +4308,12 @@
         <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>2</v>
@@ -3650,12 +4322,12 @@
         <v>24</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>2</v>
@@ -3664,89 +4336,89 @@
         <v>24</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D20" s="2">
         <v>35</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D23" s="2">
         <v>10</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
@@ -3757,13 +4429,13 @@
         <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
@@ -3774,176 +4446,176 @@
         <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D25" t="s">
         <v>64</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E26" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D34" s="2">
         <v>200</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D35" s="2">
         <v>100</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D36" s="2">
         <v>100</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.4">
@@ -3954,44 +4626,44 @@
         <v>119</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>120</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
@@ -4157,8 +4829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD63C287-BDD3-4AF4-BAC0-84A491537ABD}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46:B47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4175,7 +4847,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -4205,7 +4877,7 @@
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
@@ -4217,12 +4889,12 @@
         <v>8</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -4231,7 +4903,7 @@
         <v>117</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -4248,12 +4920,12 @@
         <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -4265,161 +4937,161 @@
         <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
@@ -4433,7 +5105,7 @@
         <v>115</v>
       </c>
       <c r="E20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -4507,10 +5179,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB419CFD-8D63-4604-B9FB-5116F92A3DFA}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4527,7 +5199,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -4535,7 +5207,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -4566,7 +5238,7 @@
         <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -4580,308 +5252,638 @@
         <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>227</v>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>212</v>
-      </c>
-      <c r="E9" t="s">
-        <v>215</v>
+        <v>235</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E10" t="s">
-        <v>216</v>
+        <v>237</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>212</v>
-      </c>
-      <c r="E11" t="s">
-        <v>217</v>
+        <v>239</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>212</v>
-      </c>
-      <c r="E12" t="s">
-        <v>218</v>
+        <v>241</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E13" t="s">
-        <v>219</v>
+        <v>242</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>212</v>
-      </c>
-      <c r="E14" t="s">
-        <v>220</v>
+        <v>245</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
+        <v>246</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E15" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>119</v>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="5" t="s">
-        <v>37</v>
+        <v>266</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+        <v>266</v>
+      </c>
+      <c r="D20" s="2">
+        <v>35</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>270</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+        <v>266</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>272</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+        <v>266</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>31</v>
+        <v>274</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+        <v>266</v>
+      </c>
+      <c r="D23" s="2">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>266</v>
       </c>
       <c r="D24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C25" t="s">
+        <v>266</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>210</v>
+      </c>
+      <c r="E26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>210</v>
+      </c>
+      <c r="E29" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>210</v>
+      </c>
+      <c r="E31" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>210</v>
+      </c>
+      <c r="E32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D34" s="2">
+        <v>200</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D35" s="2">
+        <v>100</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D36" s="2">
+        <v>100</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D25" t="s">
+      <c r="B40" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" s="2" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C46" t="s">
         <v>25</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D46" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B47" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4895,13 +5897,13 @@
           <x14:formula1>
             <xm:f>lists!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>B44:B224</xm:sqref>
+          <xm:sqref>B49:B224</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A0143D08-078D-4597-8514-5B4F5F9A50FB}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{423D77E1-2AD4-4E54-B38F-664CA3DD78A4}">
           <x14:formula1>
             <xm:f>lists!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B43</xm:sqref>
+          <xm:sqref>B5:B48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE3391A2-FF63-4508-8FED-6B395E046851}">
           <x14:formula1>
@@ -4926,7 +5928,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4943,7 +5945,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -4973,7 +5975,7 @@
     </row>
     <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
@@ -4982,15 +5984,15 @@
         <v>117</v>
       </c>
       <c r="D5" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -4999,7 +6001,7 @@
         <v>117</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -5016,12 +6018,12 @@
         <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -5033,161 +6035,161 @@
         <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
@@ -5201,7 +6203,7 @@
         <v>115</v>
       </c>
       <c r="E20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
@@ -5273,19 +6275,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664D46D0-CFAB-416B-A253-FC2929E5C79F}">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA12FDB5-27F7-4262-8C47-225F4DA5CDD3}">
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.4609375" customWidth="1"/>
+    <col min="1" max="1" width="25.921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.3046875" customWidth="1"/>
+    <col min="3" max="3" width="14.921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
@@ -5293,7 +6296,7 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -5301,7 +6304,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -5325,265 +6328,683 @@
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>266</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>266</v>
+      </c>
+      <c r="D20" s="2">
+        <v>35</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>266</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>266</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>266</v>
+      </c>
+      <c r="D23" s="2">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>266</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>266</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>210</v>
+      </c>
+      <c r="E26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>210</v>
+      </c>
+      <c r="E29" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>210</v>
+      </c>
+      <c r="E31" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>210</v>
+      </c>
+      <c r="E32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D34" s="2">
+        <v>200</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D35" s="2">
+        <v>100</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D36" s="2">
+        <v>100</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s">
         <v>105</v>
       </c>
-      <c r="E9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D42">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+      <c r="D46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B47" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
         <v>69</v>
       </c>
-      <c r="E21" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
         <v>69</v>
       </c>
-      <c r="E22" t="s">
-        <v>99</v>
-      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B49" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{592FF17C-EAEA-47DA-A2F3-BD8F9AEE7605}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CAC181C-A9E1-4E05-8CC4-5E1E695473D2}">
+          <x14:formula1>
+            <xm:f>lists!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:B64</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{63EF8F95-28C4-45D3-B538-FE81D7B070A4}">
           <x14:formula1>
             <xm:f>fields!$A$2:$A$260</xm:f>
           </x14:formula1>
-          <xm:sqref>A5:A269</xm:sqref>
+          <xm:sqref>A5:A288</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F7074770-80C9-43C1-B273-B5283AD6B093}">
-          <x14:formula1>
-            <xm:f>lists!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5:B19 B21:B22</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4A4167C6-AD91-46A4-A351-4832B091EE7E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5584AF89-DA9D-4EC8-A631-DEB72C867CA0}">
           <x14:formula1>
             <xm:f>categories!$A$2:$A$47</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C221</xm:sqref>
+          <xm:sqref>C5:C240</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{78A217F7-2DE2-45FF-81FF-3EEF5C9ED4C5}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9137E54C-0EA5-4706-AE44-E1865D757820}">
           <x14:formula1>
             <xm:f>lists!$A$2:$A$16</xm:f>
           </x14:formula1>
-          <xm:sqref>B23:B226</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A08BA68E-8F08-43D8-B97F-D9845B5C1E39}">
-          <x14:formula1>
-            <xm:f>lists!$A$2:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>B20</xm:sqref>
+          <xm:sqref>B65:B245</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>